<commit_message>
fix(general.controller): line between messages fix
</commit_message>
<xml_diff>
--- a/xlsxs/OTs data collection.xlsx
+++ b/xlsxs/OTs data collection.xlsx
@@ -8,13 +8,16 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="shitttt" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="shitttt2" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="38">
   <si>
     <t>Type of messege</t>
   </si>
@@ -34,43 +37,100 @@
     <t>feedback</t>
   </si>
   <si>
-    <t>Difficulty for young children</t>
+    <t>Amazing games</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>What a beauty!!!! Amazing games - both graphics, content, and feedback that children receive! Yesterday I tried with my 5-year-old daughter, it was difficult for her, she had to make an effort, but the satisfaction after the climb was worth the effort :).</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>Navigation game issue</t>
   </si>
   <si>
     <t>negative</t>
   </si>
   <si>
-    <t>The subject of moving only the shoulders right and left is difficult for younger children, both in terms of understanding and separating the movement.</t>
-  </si>
-  <si>
-    <t>bug</t>
-  </si>
-  <si>
-    <t>Results disappearing</t>
-  </si>
-  <si>
-    <t>The results disappeared before I could take a picture. Is it possible to go back to it?</t>
-  </si>
-  <si>
-    <t>App telling to stay in front of the camera</t>
-  </si>
-  <si>
-    <t>The app kept telling to stay in front of the camera all the time, which was a bit annoying.</t>
-  </si>
-  <si>
-    <t>Parent's excitement</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
-  <si>
-    <t>The parent was excited about the game, but also noticed the repetition of staying in front of the camera.</t>
-  </si>
-  <si>
-    <t>Game character getting lost and swapping roles</t>
-  </si>
-  <si>
-    <t>This reminds me a bit of what happened to me with one of the kids. They got lost and struggled to find their way. They were frustrated and tired with their arms. So we simply switched roles. I reached the place with the shapes and they continued with the shakshuka.</t>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect minerals when there is a note about maintaining an upright back - the correct posture window hides the path and is a bit stressful. Maybe after the initial guidance, only voice guidance would be sufficient?</t>
+  </si>
+  <si>
+    <t>Amazing games with graphics, content, and feedback</t>
+  </si>
+  <si>
+    <t>What a beauty!!!! Amazing games - both graphics, content, and feedback that children receive! Yesterday I tried with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after the climb was worth the effort :).</t>
+  </si>
+  <si>
+    <t>Issue with navigation game and collecting minerals</t>
+  </si>
+  <si>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect the minerals when a note appears to maintain a straight back - the correct posture window hides the path and is a bit stressful. Maybe after the first guidance, only a voice guidance could be sufficient?</t>
+  </si>
+  <si>
+    <t>Amazing games and graphics</t>
+  </si>
+  <si>
+    <t>What a beauty! Amazing games - graphics, content, and feedback for children! I tried it yesterday with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after the climb was worth the effort.</t>
+  </si>
+  <si>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect the minerals when there is a note about keeping a straight back - the proper posture window hides the route and is a bit stressful. Maybe after the first guidance, a voice direction would be enough?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Amazing games and positive experience</t>
+  </si>
+  <si>
+    <t>What a beauty!!!! Amazing games - both graphics, content and feedback that children receive! Yesterday I tried with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after the climb was worth the effort :).</t>
+  </si>
+  <si>
+    <t>Issue with navigation game</t>
+  </si>
+  <si>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect the minerals when a note appears about maintaining a straight back - the correct posture window hides the route and is a bit stressful. Maybe after the first guidance, only voice guidance can be sufficient?</t>
+  </si>
+  <si>
+    <t>Amazing games - graphics, content, and feedback</t>
+  </si>
+  <si>
+    <t>What a beauty!!!! Amazing games - both graphics, content, and feedback children receive! Yesterday I tried it with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after climbing was worth the effort :).</t>
+  </si>
+  <si>
+    <t>Navigation game issue with posture reminder</t>
+  </si>
+  <si>
+    <t>In the navigation game, it disturbed her and also the patients I tried with today to collect the minerals when a notice appears about keeping a straight back - the correct posture window hides the path and is a bit stressful. Maybe after the first guidance, only a vocal guidance could be sufficient?</t>
+  </si>
+  <si>
+    <t>Amazing games, graphics, and feedback</t>
+  </si>
+  <si>
+    <t>What a beauty!!!! Amazing games - both graphics, content, and feedback that children receive! Yesterday I tried it with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after the climb was worth the effort :).</t>
+  </si>
+  <si>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect minerals when a note about keeping a straight back appears - the correct posture window hides the path and is a bit stressful. Maybe after the first guidance, only voice guidance can be sufficient?</t>
+  </si>
+  <si>
+    <t>What a beauty! Amazing games - both graphics, content, and feedback kids get! Yesterday I tried it with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after the climb was worth the effort :).</t>
+  </si>
+  <si>
+    <t>Navigation issue</t>
+  </si>
+  <si>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect the minerals when a note about keeping a straight back appears - the proper posture window hides the track and is a bit stressful. Maybe after the first guidance, only vocal guidance could be sufficient?</t>
+  </si>
+  <si>
+    <t>Amazing games, graphics, content, and feedback</t>
+  </si>
+  <si>
+    <t>What a beauty!!!! Amazing games - both graphics, content and also feedback that children receive! Yesterday I tried with my 5-year-old daughter, it was hard for her, she had to make an effort, but the satisfaction after the climb was worth the effort :).</t>
+  </si>
+  <si>
+    <t>In the navigation game, it was a bit disturbing for her and also for the patients I tried with today to collect the minerals when a note about maintaining a straight back appears - the correct posture window hides the path and is a bit stressful. Maybe after the first direction, only a vocal direction could be sufficient?</t>
   </si>
 </sst>
 </file>
@@ -496,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" defaultColWidth="14.6640625" customHeight="1"/>
@@ -550,10 +610,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -561,24 +621,24 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -596,10 +656,272 @@
       </c>
       <c r="D6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
 </file>
</xml_diff>